<commit_message>
add dependency & mobile apps logs report
</commit_message>
<xml_diff>
--- a/Documents/checklist.xlsx
+++ b/Documents/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH Campus Wien\6.Semester\Bachelorarbeit 2\Arbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432D5002-A0C2-4F66-917A-DCBFFDC0511D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53FB2A4-7122-405C-90B7-B2ECCC3A065D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Security Requirements" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="286">
   <si>
     <t>Mobile Application Security Verification Standard</t>
   </si>
@@ -1098,23 +1098,23 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="6">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="7" applyAlignment="1">
       <alignment vertical="center" wrapText="1" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
       <alignment vertical="center" wrapText="1" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
@@ -1608,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Z130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I98" sqref="I98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1634,88 +1634,88 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:26" ht="64.900000000000006" customHeight="1">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:26">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="2" t="str">
         <f>HYPERLINK("https://github.com/OWASP/owasp-mastg/releases/tag/v1.5.0", "OWASP MASTG v1.5.0 (commit: 3b9278f)")</f>
         <v>OWASP MASTG v1.5.0 (commit: 3b9278f)</v>
       </c>
     </row>
     <row r="4" spans="2:26">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="2" t="str">
         <f>HYPERLINK("https://github.com/OWASP/owasp-masvs/releases/tag/v1.4.2", "OWASP MASVS v1.4.2 (commit: 2a8b582)")</f>
         <v>OWASP MASVS v1.4.2 (commit: 2a8b582)</v>
       </c>
     </row>
     <row r="7" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="12"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
     </row>
     <row r="8" spans="2:26" ht="70.150000000000006" customHeight="1">
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="13" t="s">
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="15" t="s">
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="13" t="s">
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="15" t="s">
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="13" t="s">
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
     </row>
     <row r="10" spans="2:26">
       <c r="B10" s="3" t="s">
@@ -2043,33 +2043,33 @@
     </row>
     <row r="24" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="25" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="12"/>
-      <c r="S25" s="12"/>
-      <c r="T25" s="12"/>
-      <c r="U25" s="12"/>
-      <c r="V25" s="12"/>
-      <c r="W25" s="12"/>
-      <c r="X25" s="12"/>
-      <c r="Y25" s="12"/>
-      <c r="Z25" s="12"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
     </row>
     <row r="27" spans="2:26">
       <c r="B27" s="3" t="s">
@@ -2556,33 +2556,33 @@
     </row>
     <row r="44" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="45" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
-      <c r="P45" s="12"/>
-      <c r="Q45" s="12"/>
-      <c r="R45" s="12"/>
-      <c r="S45" s="12"/>
-      <c r="T45" s="12"/>
-      <c r="U45" s="12"/>
-      <c r="V45" s="12"/>
-      <c r="W45" s="12"/>
-      <c r="X45" s="12"/>
-      <c r="Y45" s="12"/>
-      <c r="Z45" s="12"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11"/>
+      <c r="U45" s="11"/>
+      <c r="V45" s="11"/>
+      <c r="W45" s="11"/>
+      <c r="X45" s="11"/>
+      <c r="Y45" s="11"/>
+      <c r="Z45" s="11"/>
     </row>
     <row r="47" spans="2:26">
       <c r="B47" s="3" t="s">
@@ -2868,33 +2868,33 @@
     </row>
     <row r="55" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="56" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="12"/>
-      <c r="L56" s="12"/>
-      <c r="M56" s="12"/>
-      <c r="N56" s="12"/>
-      <c r="O56" s="12"/>
-      <c r="P56" s="12"/>
-      <c r="Q56" s="12"/>
-      <c r="R56" s="12"/>
-      <c r="S56" s="12"/>
-      <c r="T56" s="12"/>
-      <c r="U56" s="12"/>
-      <c r="V56" s="12"/>
-      <c r="W56" s="12"/>
-      <c r="X56" s="12"/>
-      <c r="Y56" s="12"/>
-      <c r="Z56" s="12"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
+      <c r="T56" s="11"/>
+      <c r="U56" s="11"/>
+      <c r="V56" s="11"/>
+      <c r="W56" s="11"/>
+      <c r="X56" s="11"/>
+      <c r="Y56" s="11"/>
+      <c r="Z56" s="11"/>
     </row>
     <row r="58" spans="2:26">
       <c r="B58" s="3" t="s">
@@ -3282,33 +3282,33 @@
     </row>
     <row r="72" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="73" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="12"/>
-      <c r="I73" s="12"/>
-      <c r="J73" s="12"/>
-      <c r="K73" s="12"/>
-      <c r="L73" s="12"/>
-      <c r="M73" s="12"/>
-      <c r="N73" s="12"/>
-      <c r="O73" s="12"/>
-      <c r="P73" s="12"/>
-      <c r="Q73" s="12"/>
-      <c r="R73" s="12"/>
-      <c r="S73" s="12"/>
-      <c r="T73" s="12"/>
-      <c r="U73" s="12"/>
-      <c r="V73" s="12"/>
-      <c r="W73" s="12"/>
-      <c r="X73" s="12"/>
-      <c r="Y73" s="12"/>
-      <c r="Z73" s="12"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="11"/>
+      <c r="K73" s="11"/>
+      <c r="L73" s="11"/>
+      <c r="M73" s="11"/>
+      <c r="N73" s="11"/>
+      <c r="O73" s="11"/>
+      <c r="P73" s="11"/>
+      <c r="Q73" s="11"/>
+      <c r="R73" s="11"/>
+      <c r="S73" s="11"/>
+      <c r="T73" s="11"/>
+      <c r="U73" s="11"/>
+      <c r="V73" s="11"/>
+      <c r="W73" s="11"/>
+      <c r="X73" s="11"/>
+      <c r="Y73" s="11"/>
+      <c r="Z73" s="11"/>
     </row>
     <row r="75" spans="2:26">
       <c r="B75" s="3" t="s">
@@ -3564,33 +3564,33 @@
     </row>
     <row r="83" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="84" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B84" s="11" t="s">
+      <c r="B84" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="12"/>
-      <c r="I84" s="12"/>
-      <c r="J84" s="12"/>
-      <c r="K84" s="12"/>
-      <c r="L84" s="12"/>
-      <c r="M84" s="12"/>
-      <c r="N84" s="12"/>
-      <c r="O84" s="12"/>
-      <c r="P84" s="12"/>
-      <c r="Q84" s="12"/>
-      <c r="R84" s="12"/>
-      <c r="S84" s="12"/>
-      <c r="T84" s="12"/>
-      <c r="U84" s="12"/>
-      <c r="V84" s="12"/>
-      <c r="W84" s="12"/>
-      <c r="X84" s="12"/>
-      <c r="Y84" s="12"/>
-      <c r="Z84" s="12"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="11"/>
+      <c r="H84" s="11"/>
+      <c r="I84" s="11"/>
+      <c r="J84" s="11"/>
+      <c r="K84" s="11"/>
+      <c r="L84" s="11"/>
+      <c r="M84" s="11"/>
+      <c r="N84" s="11"/>
+      <c r="O84" s="11"/>
+      <c r="P84" s="11"/>
+      <c r="Q84" s="11"/>
+      <c r="R84" s="11"/>
+      <c r="S84" s="11"/>
+      <c r="T84" s="11"/>
+      <c r="U84" s="11"/>
+      <c r="V84" s="11"/>
+      <c r="W84" s="11"/>
+      <c r="X84" s="11"/>
+      <c r="Y84" s="11"/>
+      <c r="Z84" s="11"/>
     </row>
     <row r="86" spans="2:26">
       <c r="B86" s="3" t="s">
@@ -3989,33 +3989,33 @@
     </row>
     <row r="99" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="100" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B100" s="11" t="s">
+      <c r="B100" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="C100" s="12"/>
-      <c r="D100" s="12"/>
-      <c r="E100" s="12"/>
-      <c r="F100" s="12"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="12"/>
-      <c r="I100" s="12"/>
-      <c r="J100" s="12"/>
-      <c r="K100" s="12"/>
-      <c r="L100" s="12"/>
-      <c r="M100" s="12"/>
-      <c r="N100" s="12"/>
-      <c r="O100" s="12"/>
-      <c r="P100" s="12"/>
-      <c r="Q100" s="12"/>
-      <c r="R100" s="12"/>
-      <c r="S100" s="12"/>
-      <c r="T100" s="12"/>
-      <c r="U100" s="12"/>
-      <c r="V100" s="12"/>
-      <c r="W100" s="12"/>
-      <c r="X100" s="12"/>
-      <c r="Y100" s="12"/>
-      <c r="Z100" s="12"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="11"/>
+      <c r="E100" s="11"/>
+      <c r="F100" s="11"/>
+      <c r="G100" s="11"/>
+      <c r="H100" s="11"/>
+      <c r="I100" s="11"/>
+      <c r="J100" s="11"/>
+      <c r="K100" s="11"/>
+      <c r="L100" s="11"/>
+      <c r="M100" s="11"/>
+      <c r="N100" s="11"/>
+      <c r="O100" s="11"/>
+      <c r="P100" s="11"/>
+      <c r="Q100" s="11"/>
+      <c r="R100" s="11"/>
+      <c r="S100" s="11"/>
+      <c r="T100" s="11"/>
+      <c r="U100" s="11"/>
+      <c r="V100" s="11"/>
+      <c r="W100" s="11"/>
+      <c r="X100" s="11"/>
+      <c r="Y100" s="11"/>
+      <c r="Z100" s="11"/>
     </row>
     <row r="102" spans="2:26">
       <c r="B102" s="3" t="s">
@@ -4243,9 +4243,7 @@
       <c r="L108" s="7"/>
       <c r="N108" s="6"/>
       <c r="O108" s="7"/>
-      <c r="Q108" s="6" t="s">
-        <v>281</v>
-      </c>
+      <c r="Q108" s="6"/>
       <c r="R108" s="7"/>
       <c r="T108" s="6"/>
       <c r="U108" s="7"/>
@@ -4384,33 +4382,33 @@
     </row>
     <row r="113" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="114" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B114" s="11" t="s">
+      <c r="B114" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="C114" s="12"/>
-      <c r="D114" s="12"/>
-      <c r="E114" s="12"/>
-      <c r="F114" s="12"/>
-      <c r="G114" s="12"/>
-      <c r="H114" s="12"/>
-      <c r="I114" s="12"/>
-      <c r="J114" s="12"/>
-      <c r="K114" s="12"/>
-      <c r="L114" s="12"/>
-      <c r="M114" s="12"/>
-      <c r="N114" s="12"/>
-      <c r="O114" s="12"/>
-      <c r="P114" s="12"/>
-      <c r="Q114" s="12"/>
-      <c r="R114" s="12"/>
-      <c r="S114" s="12"/>
-      <c r="T114" s="12"/>
-      <c r="U114" s="12"/>
-      <c r="V114" s="12"/>
-      <c r="W114" s="12"/>
-      <c r="X114" s="12"/>
-      <c r="Y114" s="12"/>
-      <c r="Z114" s="12"/>
+      <c r="C114" s="11"/>
+      <c r="D114" s="11"/>
+      <c r="E114" s="11"/>
+      <c r="F114" s="11"/>
+      <c r="G114" s="11"/>
+      <c r="H114" s="11"/>
+      <c r="I114" s="11"/>
+      <c r="J114" s="11"/>
+      <c r="K114" s="11"/>
+      <c r="L114" s="11"/>
+      <c r="M114" s="11"/>
+      <c r="N114" s="11"/>
+      <c r="O114" s="11"/>
+      <c r="P114" s="11"/>
+      <c r="Q114" s="11"/>
+      <c r="R114" s="11"/>
+      <c r="S114" s="11"/>
+      <c r="T114" s="11"/>
+      <c r="U114" s="11"/>
+      <c r="V114" s="11"/>
+      <c r="W114" s="11"/>
+      <c r="X114" s="11"/>
+      <c r="Y114" s="11"/>
+      <c r="Z114" s="11"/>
     </row>
     <row r="116" spans="2:26">
       <c r="B116" s="3" t="s">
@@ -4779,6 +4777,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B2:C4"/>
+    <mergeCell ref="B7:Z7"/>
+    <mergeCell ref="B25:Z25"/>
+    <mergeCell ref="B45:Z45"/>
+    <mergeCell ref="B56:Z56"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="Q8:S8"/>
     <mergeCell ref="B73:Z73"/>
     <mergeCell ref="B84:Z84"/>
     <mergeCell ref="B100:Z100"/>
@@ -4787,13 +4792,6 @@
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="K8:M8"/>
     <mergeCell ref="N8:P8"/>
-    <mergeCell ref="B2:C4"/>
-    <mergeCell ref="B7:Z7"/>
-    <mergeCell ref="B25:Z25"/>
-    <mergeCell ref="B45:Z45"/>
-    <mergeCell ref="B56:Z56"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="Q8:S8"/>
   </mergeCells>
   <conditionalFormatting sqref="Z12:Z401">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Fail">
@@ -4812,7 +4810,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4832,55 +4831,55 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="64.900000000000006" customHeight="1">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="2" t="str">
         <f>HYPERLINK("https://github.com/OWASP/owasp-mastg/releases/tag/v1.5.0", "OWASP MASTG v1.5.0 (commit: 3b9278f)")</f>
         <v>OWASP MASTG v1.5.0 (commit: 3b9278f)</v>
       </c>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="2" t="str">
         <f>HYPERLINK("https://github.com/OWASP/owasp-masvs/releases/tag/v1.4.2", "OWASP MASVS v1.4.2 (commit: 2a8b582)")</f>
         <v>OWASP MASVS v1.4.2 (commit: 2a8b582)</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="25.15" customHeight="1">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
     </row>
     <row r="12" spans="2:11">
       <c r="B12" t="str">
@@ -4892,15 +4891,15 @@
       <c r="B14" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" t="str">
@@ -4912,15 +4911,15 @@
       <c r="B18" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
     </row>
     <row r="20" spans="2:11">
       <c r="B20" t="str">
@@ -4929,32 +4928,32 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="25.15" customHeight="1">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
     </row>
     <row r="24" spans="2:11">
       <c r="B24" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
     </row>
     <row r="26" spans="2:11">
       <c r="B26" t="str">
@@ -4963,32 +4962,32 @@
       </c>
     </row>
     <row r="28" spans="2:11" ht="25.15" customHeight="1">
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
     </row>
     <row r="30" spans="2:11">
       <c r="B30" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
     </row>
     <row r="32" spans="2:11">
       <c r="B32" t="str">

</xml_diff>

<commit_message>
update MAS checklist & add mobile apps logs report
</commit_message>
<xml_diff>
--- a/Documents/checklist.xlsx
+++ b/Documents/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH Campus Wien\6.Semester\Bachelorarbeit 2\Arbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53FB2A4-7122-405C-90B7-B2ECCC3A065D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D533C6CE-D99E-457B-AB0A-8AC7249219D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="286">
   <si>
     <t>Mobile Application Security Verification Standard</t>
   </si>
@@ -1098,23 +1098,23 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="6">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="7" applyAlignment="1">
       <alignment vertical="center" wrapText="1" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
       <alignment vertical="center" wrapText="1" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
@@ -1608,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Z130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I98" sqref="I98"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1634,88 +1634,88 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:26" ht="64.900000000000006" customHeight="1">
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:26">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="2" t="str">
         <f>HYPERLINK("https://github.com/OWASP/owasp-mastg/releases/tag/v1.5.0", "OWASP MASTG v1.5.0 (commit: 3b9278f)")</f>
         <v>OWASP MASTG v1.5.0 (commit: 3b9278f)</v>
       </c>
     </row>
     <row r="4" spans="2:26">
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="2" t="str">
         <f>HYPERLINK("https://github.com/OWASP/owasp-masvs/releases/tag/v1.4.2", "OWASP MASVS v1.4.2 (commit: 2a8b582)")</f>
         <v>OWASP MASVS v1.4.2 (commit: 2a8b582)</v>
       </c>
     </row>
     <row r="7" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
     </row>
     <row r="8" spans="2:26" ht="70.150000000000006" customHeight="1">
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14" t="s">
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="12" t="s">
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="14" t="s">
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="12" t="s">
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="14" t="s">
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
     </row>
     <row r="10" spans="2:26">
       <c r="B10" s="3" t="s">
@@ -2043,33 +2043,33 @@
     </row>
     <row r="24" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="25" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="11"/>
-      <c r="Z25" s="11"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="12"/>
+      <c r="Y25" s="12"/>
+      <c r="Z25" s="12"/>
     </row>
     <row r="27" spans="2:26">
       <c r="B27" s="3" t="s">
@@ -2194,9 +2194,7 @@
       <c r="F30" s="7"/>
       <c r="H30" s="6"/>
       <c r="I30" s="7"/>
-      <c r="K30" s="6" t="s">
-        <v>281</v>
-      </c>
+      <c r="K30" s="6"/>
       <c r="L30" s="7"/>
       <c r="N30" s="6"/>
       <c r="O30" s="7"/>
@@ -2556,33 +2554,33 @@
     </row>
     <row r="44" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="45" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-      <c r="S45" s="11"/>
-      <c r="T45" s="11"/>
-      <c r="U45" s="11"/>
-      <c r="V45" s="11"/>
-      <c r="W45" s="11"/>
-      <c r="X45" s="11"/>
-      <c r="Y45" s="11"/>
-      <c r="Z45" s="11"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
+      <c r="S45" s="12"/>
+      <c r="T45" s="12"/>
+      <c r="U45" s="12"/>
+      <c r="V45" s="12"/>
+      <c r="W45" s="12"/>
+      <c r="X45" s="12"/>
+      <c r="Y45" s="12"/>
+      <c r="Z45" s="12"/>
     </row>
     <row r="47" spans="2:26">
       <c r="B47" s="3" t="s">
@@ -2868,33 +2866,33 @@
     </row>
     <row r="55" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="56" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="11"/>
-      <c r="L56" s="11"/>
-      <c r="M56" s="11"/>
-      <c r="N56" s="11"/>
-      <c r="O56" s="11"/>
-      <c r="P56" s="11"/>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="11"/>
-      <c r="S56" s="11"/>
-      <c r="T56" s="11"/>
-      <c r="U56" s="11"/>
-      <c r="V56" s="11"/>
-      <c r="W56" s="11"/>
-      <c r="X56" s="11"/>
-      <c r="Y56" s="11"/>
-      <c r="Z56" s="11"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
+      <c r="L56" s="12"/>
+      <c r="M56" s="12"/>
+      <c r="N56" s="12"/>
+      <c r="O56" s="12"/>
+      <c r="P56" s="12"/>
+      <c r="Q56" s="12"/>
+      <c r="R56" s="12"/>
+      <c r="S56" s="12"/>
+      <c r="T56" s="12"/>
+      <c r="U56" s="12"/>
+      <c r="V56" s="12"/>
+      <c r="W56" s="12"/>
+      <c r="X56" s="12"/>
+      <c r="Y56" s="12"/>
+      <c r="Z56" s="12"/>
     </row>
     <row r="58" spans="2:26">
       <c r="B58" s="3" t="s">
@@ -3282,33 +3280,33 @@
     </row>
     <row r="72" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="73" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B73" s="10" t="s">
+      <c r="B73" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
-      <c r="I73" s="11"/>
-      <c r="J73" s="11"/>
-      <c r="K73" s="11"/>
-      <c r="L73" s="11"/>
-      <c r="M73" s="11"/>
-      <c r="N73" s="11"/>
-      <c r="O73" s="11"/>
-      <c r="P73" s="11"/>
-      <c r="Q73" s="11"/>
-      <c r="R73" s="11"/>
-      <c r="S73" s="11"/>
-      <c r="T73" s="11"/>
-      <c r="U73" s="11"/>
-      <c r="V73" s="11"/>
-      <c r="W73" s="11"/>
-      <c r="X73" s="11"/>
-      <c r="Y73" s="11"/>
-      <c r="Z73" s="11"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="12"/>
+      <c r="J73" s="12"/>
+      <c r="K73" s="12"/>
+      <c r="L73" s="12"/>
+      <c r="M73" s="12"/>
+      <c r="N73" s="12"/>
+      <c r="O73" s="12"/>
+      <c r="P73" s="12"/>
+      <c r="Q73" s="12"/>
+      <c r="R73" s="12"/>
+      <c r="S73" s="12"/>
+      <c r="T73" s="12"/>
+      <c r="U73" s="12"/>
+      <c r="V73" s="12"/>
+      <c r="W73" s="12"/>
+      <c r="X73" s="12"/>
+      <c r="Y73" s="12"/>
+      <c r="Z73" s="12"/>
     </row>
     <row r="75" spans="2:26">
       <c r="B75" s="3" t="s">
@@ -3564,33 +3562,33 @@
     </row>
     <row r="83" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="84" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B84" s="10" t="s">
+      <c r="B84" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
-      <c r="F84" s="11"/>
-      <c r="G84" s="11"/>
-      <c r="H84" s="11"/>
-      <c r="I84" s="11"/>
-      <c r="J84" s="11"/>
-      <c r="K84" s="11"/>
-      <c r="L84" s="11"/>
-      <c r="M84" s="11"/>
-      <c r="N84" s="11"/>
-      <c r="O84" s="11"/>
-      <c r="P84" s="11"/>
-      <c r="Q84" s="11"/>
-      <c r="R84" s="11"/>
-      <c r="S84" s="11"/>
-      <c r="T84" s="11"/>
-      <c r="U84" s="11"/>
-      <c r="V84" s="11"/>
-      <c r="W84" s="11"/>
-      <c r="X84" s="11"/>
-      <c r="Y84" s="11"/>
-      <c r="Z84" s="11"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="12"/>
+      <c r="K84" s="12"/>
+      <c r="L84" s="12"/>
+      <c r="M84" s="12"/>
+      <c r="N84" s="12"/>
+      <c r="O84" s="12"/>
+      <c r="P84" s="12"/>
+      <c r="Q84" s="12"/>
+      <c r="R84" s="12"/>
+      <c r="S84" s="12"/>
+      <c r="T84" s="12"/>
+      <c r="U84" s="12"/>
+      <c r="V84" s="12"/>
+      <c r="W84" s="12"/>
+      <c r="X84" s="12"/>
+      <c r="Y84" s="12"/>
+      <c r="Z84" s="12"/>
     </row>
     <row r="86" spans="2:26">
       <c r="B86" s="3" t="s">
@@ -3989,33 +3987,33 @@
     </row>
     <row r="99" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="100" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B100" s="10" t="s">
+      <c r="B100" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="C100" s="11"/>
-      <c r="D100" s="11"/>
-      <c r="E100" s="11"/>
-      <c r="F100" s="11"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="11"/>
-      <c r="I100" s="11"/>
-      <c r="J100" s="11"/>
-      <c r="K100" s="11"/>
-      <c r="L100" s="11"/>
-      <c r="M100" s="11"/>
-      <c r="N100" s="11"/>
-      <c r="O100" s="11"/>
-      <c r="P100" s="11"/>
-      <c r="Q100" s="11"/>
-      <c r="R100" s="11"/>
-      <c r="S100" s="11"/>
-      <c r="T100" s="11"/>
-      <c r="U100" s="11"/>
-      <c r="V100" s="11"/>
-      <c r="W100" s="11"/>
-      <c r="X100" s="11"/>
-      <c r="Y100" s="11"/>
-      <c r="Z100" s="11"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
+      <c r="H100" s="12"/>
+      <c r="I100" s="12"/>
+      <c r="J100" s="12"/>
+      <c r="K100" s="12"/>
+      <c r="L100" s="12"/>
+      <c r="M100" s="12"/>
+      <c r="N100" s="12"/>
+      <c r="O100" s="12"/>
+      <c r="P100" s="12"/>
+      <c r="Q100" s="12"/>
+      <c r="R100" s="12"/>
+      <c r="S100" s="12"/>
+      <c r="T100" s="12"/>
+      <c r="U100" s="12"/>
+      <c r="V100" s="12"/>
+      <c r="W100" s="12"/>
+      <c r="X100" s="12"/>
+      <c r="Y100" s="12"/>
+      <c r="Z100" s="12"/>
     </row>
     <row r="102" spans="2:26">
       <c r="B102" s="3" t="s">
@@ -4382,33 +4380,33 @@
     </row>
     <row r="113" spans="2:26" ht="15.75" thickTop="1"/>
     <row r="114" spans="2:26" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B114" s="10" t="s">
+      <c r="B114" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11"/>
-      <c r="F114" s="11"/>
-      <c r="G114" s="11"/>
-      <c r="H114" s="11"/>
-      <c r="I114" s="11"/>
-      <c r="J114" s="11"/>
-      <c r="K114" s="11"/>
-      <c r="L114" s="11"/>
-      <c r="M114" s="11"/>
-      <c r="N114" s="11"/>
-      <c r="O114" s="11"/>
-      <c r="P114" s="11"/>
-      <c r="Q114" s="11"/>
-      <c r="R114" s="11"/>
-      <c r="S114" s="11"/>
-      <c r="T114" s="11"/>
-      <c r="U114" s="11"/>
-      <c r="V114" s="11"/>
-      <c r="W114" s="11"/>
-      <c r="X114" s="11"/>
-      <c r="Y114" s="11"/>
-      <c r="Z114" s="11"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
+      <c r="G114" s="12"/>
+      <c r="H114" s="12"/>
+      <c r="I114" s="12"/>
+      <c r="J114" s="12"/>
+      <c r="K114" s="12"/>
+      <c r="L114" s="12"/>
+      <c r="M114" s="12"/>
+      <c r="N114" s="12"/>
+      <c r="O114" s="12"/>
+      <c r="P114" s="12"/>
+      <c r="Q114" s="12"/>
+      <c r="R114" s="12"/>
+      <c r="S114" s="12"/>
+      <c r="T114" s="12"/>
+      <c r="U114" s="12"/>
+      <c r="V114" s="12"/>
+      <c r="W114" s="12"/>
+      <c r="X114" s="12"/>
+      <c r="Y114" s="12"/>
+      <c r="Z114" s="12"/>
     </row>
     <row r="116" spans="2:26">
       <c r="B116" s="3" t="s">
@@ -4777,13 +4775,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B2:C4"/>
-    <mergeCell ref="B7:Z7"/>
-    <mergeCell ref="B25:Z25"/>
-    <mergeCell ref="B45:Z45"/>
-    <mergeCell ref="B56:Z56"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="Q8:S8"/>
     <mergeCell ref="B73:Z73"/>
     <mergeCell ref="B84:Z84"/>
     <mergeCell ref="B100:Z100"/>
@@ -4792,6 +4783,13 @@
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="K8:M8"/>
     <mergeCell ref="N8:P8"/>
+    <mergeCell ref="B2:C4"/>
+    <mergeCell ref="B7:Z7"/>
+    <mergeCell ref="B25:Z25"/>
+    <mergeCell ref="B45:Z45"/>
+    <mergeCell ref="B56:Z56"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="Q8:S8"/>
   </mergeCells>
   <conditionalFormatting sqref="Z12:Z401">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Fail">
@@ -4831,55 +4829,55 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="64.900000000000006" customHeight="1">
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="2" t="str">
         <f>HYPERLINK("https://github.com/OWASP/owasp-mastg/releases/tag/v1.5.0", "OWASP MASTG v1.5.0 (commit: 3b9278f)")</f>
         <v>OWASP MASTG v1.5.0 (commit: 3b9278f)</v>
       </c>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="2" t="str">
         <f>HYPERLINK("https://github.com/OWASP/owasp-masvs/releases/tag/v1.4.2", "OWASP MASVS v1.4.2 (commit: 2a8b582)")</f>
         <v>OWASP MASVS v1.4.2 (commit: 2a8b582)</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="25.15" customHeight="1">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
     </row>
     <row r="12" spans="2:11">
       <c r="B12" t="str">
@@ -4891,15 +4889,15 @@
       <c r="B14" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" t="str">
@@ -4911,15 +4909,15 @@
       <c r="B18" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
     </row>
     <row r="20" spans="2:11">
       <c r="B20" t="str">
@@ -4928,32 +4926,32 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="25.15" customHeight="1">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
     </row>
     <row r="24" spans="2:11">
       <c r="B24" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
     </row>
     <row r="26" spans="2:11">
       <c r="B26" t="str">
@@ -4962,32 +4960,32 @@
       </c>
     </row>
     <row r="28" spans="2:11" ht="25.15" customHeight="1">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
     </row>
     <row r="30" spans="2:11">
       <c r="B30" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
     </row>
     <row r="32" spans="2:11">
       <c r="B32" t="str">

</xml_diff>